<commit_message>
Updated project to parse new input excel file.
</commit_message>
<xml_diff>
--- a/input/Docks_Consumption.xlsx
+++ b/input/Docks_Consumption.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935"/>
   </bookViews>
   <sheets>
-    <sheet name="October" sheetId="2" r:id="rId1"/>
-    <sheet name="September" sheetId="4" r:id="rId2"/>
-    <sheet name="August" sheetId="5" r:id="rId3"/>
-    <sheet name="July" sheetId="6" r:id="rId4"/>
-    <sheet name="June" sheetId="7" r:id="rId5"/>
-    <sheet name="May" sheetId="8" r:id="rId6"/>
-    <sheet name="April" sheetId="9" r:id="rId7"/>
-    <sheet name="March" sheetId="10" r:id="rId8"/>
-    <sheet name="February" sheetId="3" r:id="rId9"/>
-    <sheet name="January" sheetId="1" r:id="rId10"/>
-    <sheet name="December" sheetId="11" r:id="rId11"/>
-    <sheet name="November" sheetId="12" r:id="rId12"/>
+    <sheet name="10_2016" sheetId="2" r:id="rId1"/>
+    <sheet name="9_2016" sheetId="4" r:id="rId2"/>
+    <sheet name="8_2016" sheetId="5" r:id="rId3"/>
+    <sheet name="7_2016" sheetId="6" r:id="rId4"/>
+    <sheet name="6_2016" sheetId="7" r:id="rId5"/>
+    <sheet name="5_2016" sheetId="8" r:id="rId6"/>
+    <sheet name="4_2016" sheetId="9" r:id="rId7"/>
+    <sheet name="3_2016" sheetId="10" r:id="rId8"/>
+    <sheet name="2_2016" sheetId="3" r:id="rId9"/>
+    <sheet name="1_2016" sheetId="1" r:id="rId10"/>
+    <sheet name="12_2015" sheetId="11" r:id="rId11"/>
+    <sheet name="11_2015" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,18 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="17">
-  <si>
-    <t>Heat (MWH)</t>
-  </si>
-  <si>
-    <t>Hot_Water (m3)</t>
-  </si>
-  <si>
-    <t>Cold_Water (m3)</t>
-  </si>
-  <si>
-    <t>Electricity (KWH)</t>
-  </si>
   <si>
     <t>IGN_BATIMENT0000000113477385</t>
   </si>
@@ -86,6 +74,18 @@
   </si>
   <si>
     <t>GMLID</t>
+  </si>
+  <si>
+    <t>Electricity_KWH</t>
+  </si>
+  <si>
+    <t>Cold_Water_m3</t>
+  </si>
+  <si>
+    <t>Hot_Water_m3</t>
+  </si>
+  <si>
+    <t>Heat_MWH</t>
   </si>
 </sst>
 </file>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,24 +440,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>6787</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>7698</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>6954</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>14358</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>15421</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>15682</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>13859</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>12098</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>18128</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>12396</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>12089</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>18596</v>
@@ -673,31 +673,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>10850</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>11882</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>10985</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>23646</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>24623</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>24856</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>23589</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>21498</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>25925</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>21603</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>19256</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>26832</v>
@@ -901,6 +901,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -909,31 +910,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>9797</v>
@@ -950,7 +951,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>10697</v>
@@ -967,7 +968,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>10069</v>
@@ -984,7 +985,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>21938</v>
@@ -1001,7 +1002,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>21903</v>
@@ -1018,7 +1019,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>22231</v>
@@ -1035,7 +1036,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>21498</v>
@@ -1052,7 +1053,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>18898</v>
@@ -1069,7 +1070,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>23210</v>
@@ -1086,7 +1087,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>19503</v>
@@ -1103,7 +1104,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>17396</v>
@@ -1120,7 +1121,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>23985</v>
@@ -1137,6 +1138,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1145,7 +1147,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,24 +1157,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>7598</v>
@@ -1189,7 +1191,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>8496</v>
@@ -1206,7 +1208,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>7885</v>
@@ -1223,7 +1225,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>17696</v>
@@ -1240,7 +1242,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>18769</v>
@@ -1257,7 +1259,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>19002</v>
@@ -1274,7 +1276,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>17059</v>
@@ -1291,7 +1293,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>15074</v>
@@ -1308,7 +1310,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>20629</v>
@@ -1325,7 +1327,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>15249</v>
@@ -1342,7 +1344,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>15514</v>
@@ -1359,7 +1361,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>21231</v>
@@ -1376,6 +1378,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1383,32 +1386,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>5509</v>
@@ -1425,7 +1428,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>6654</v>
@@ -1442,7 +1445,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>6389</v>
@@ -1459,7 +1462,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>12112</v>
@@ -1476,7 +1479,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>13259</v>
@@ -1493,7 +1496,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>13597</v>
@@ -1510,7 +1513,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>11598</v>
@@ -1527,7 +1530,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>11194</v>
@@ -1544,7 +1547,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>15520</v>
@@ -1561,7 +1564,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>10026</v>
@@ -1578,7 +1581,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>9652</v>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>16267</v>
@@ -1620,31 +1623,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>2587</v>
@@ -1661,7 +1664,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>3529</v>
@@ -1678,7 +1681,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>2810</v>
@@ -1695,7 +1698,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>7287</v>
@@ -1712,7 +1715,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>7801</v>
@@ -1729,7 +1732,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>8264</v>
@@ -1746,7 +1749,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>6921</v>
@@ -1763,7 +1766,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>4028</v>
@@ -1780,7 +1783,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>6123</v>
@@ -1797,7 +1800,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>5365</v>
@@ -1814,7 +1817,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>2889</v>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>7896</v>
@@ -1856,31 +1859,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>3298</v>
@@ -1897,7 +1900,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>4084</v>
@@ -1914,7 +1917,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>3385</v>
@@ -1931,7 +1934,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>8628</v>
@@ -1948,7 +1951,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>9602</v>
@@ -1965,7 +1968,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>9992</v>
@@ -1982,7 +1985,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>8169</v>
@@ -1999,7 +2002,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>5597</v>
@@ -2016,7 +2019,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>9216</v>
@@ -2033,7 +2036,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>6765</v>
@@ -2050,7 +2053,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>4423</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>10298</v>
@@ -2092,31 +2095,34 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>4159</v>
@@ -2133,7 +2139,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>5102</v>
@@ -2150,7 +2156,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>4395</v>
@@ -2167,7 +2173,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>11359</v>
@@ -2184,7 +2190,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>12325</v>
@@ -2201,7 +2207,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>12759</v>
@@ -2218,7 +2224,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>10759</v>
@@ -2235,7 +2241,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>8279</v>
@@ -2252,7 +2258,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>13016</v>
@@ -2269,7 +2275,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>9365</v>
@@ -2286,7 +2292,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>7162</v>
@@ -2303,7 +2309,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>15002</v>
@@ -2328,7 +2334,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,24 +2344,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>5954</v>
@@ -2372,7 +2378,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>6889</v>
@@ -2389,7 +2395,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>6128</v>
@@ -2406,7 +2412,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>14269</v>
@@ -2423,7 +2429,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>15212</v>
@@ -2440,7 +2446,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>15503</v>
@@ -2457,7 +2463,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>13864</v>
@@ -2474,7 +2480,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>11299</v>
@@ -2491,7 +2497,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>15823</v>
@@ -2508,7 +2514,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>12028</v>
@@ -2525,7 +2531,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>10256</v>
@@ -2542,7 +2548,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>16493</v>
@@ -2567,31 +2573,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>7128</v>
@@ -2608,7 +2614,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>7969</v>
@@ -2625,7 +2631,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>7302</v>
@@ -2642,7 +2648,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>16389</v>
@@ -2659,7 +2665,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>17060</v>
@@ -2676,7 +2682,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>17264</v>
@@ -2693,7 +2699,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>15526</v>
@@ -2710,7 +2716,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>14038</v>
@@ -2727,7 +2733,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>19024</v>
@@ -2744,7 +2750,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>13836</v>
@@ -2761,7 +2767,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>12859</v>
@@ -2778,7 +2784,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>20569</v>
@@ -2803,31 +2809,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>8597</v>
@@ -2844,7 +2850,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>9723</v>
@@ -2861,7 +2867,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>8864</v>
@@ -2878,7 +2884,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>19093</v>
@@ -2895,7 +2901,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>20098</v>
@@ -2912,7 +2918,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>20264</v>
@@ -2929,7 +2935,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>18529</v>
@@ -2946,7 +2952,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>16199</v>
@@ -2963,7 +2969,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>21526</v>
@@ -2980,7 +2986,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>16821</v>
@@ -2997,7 +3003,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>15123</v>
@@ -3014,7 +3020,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>22569</v>
@@ -3039,31 +3045,31 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="A1:E13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>10159</v>
@@ -3080,7 +3086,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>11387</v>
@@ -3097,7 +3103,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>10459</v>
@@ -3114,7 +3120,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>22184</v>
@@ -3131,7 +3137,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>23189</v>
@@ -3148,7 +3154,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>23421</v>
@@ -3165,7 +3171,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>21789</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>19789</v>
@@ -3199,7 +3205,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>25126</v>
@@ -3216,7 +3222,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>20485</v>
@@ -3233,7 +3239,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>18636</v>
@@ -3250,7 +3256,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>26998</v>

</xml_diff>